<commit_message>
Added seperate HTML and saving between starting functions using excel
</commit_message>
<xml_diff>
--- a/main/sentences.xlsx
+++ b/main/sentences.xlsx
@@ -8,19 +8,30 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sentences" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
-  <si>
-    <t xml:space="preserve">hello </t>
-  </si>
-  <si>
-    <t>what is this</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <si>
+    <t>test three</t>
+  </si>
+  <si>
+    <t>test four</t>
+  </si>
+  <si>
+    <t>test five</t>
+  </si>
+  <si>
+    <t>test six</t>
+  </si>
+  <si>
+    <t>test seven</t>
+  </si>
+  <si>
+    <t>test eight</t>
   </si>
 </sst>
 </file>
@@ -329,16 +340,6 @@
     <sheetView tabSelected="true" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
@@ -350,6 +351,26 @@
         <v>1</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
 </worksheet>
 </file>
</xml_diff>